<commit_message>
Fix power LED value
</commit_message>
<xml_diff>
--- a/XUF208_Breakout_BOM.xlsx
+++ b/XUF208_Breakout_BOM.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
   <si>
     <t>Quantity</t>
   </si>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t>R9</t>
-  </si>
-  <si>
-    <t>220</t>
   </si>
   <si>
     <t>RC0603FR-07220RL</t>
@@ -480,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -494,6 +491,9 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1137,8 +1137,8 @@
       <c r="B19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>78</v>
+      <c r="C19" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>58</v>
@@ -1147,7 +1147,7 @@
         <v>59</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>61</v>
@@ -1158,10 +1158,10 @@
         <v>1.0</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>58</v>
@@ -1170,7 +1170,7 @@
         <v>59</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>61</v>
@@ -1181,10 +1181,10 @@
         <v>1.0</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>58</v>
@@ -1193,7 +1193,7 @@
         <v>59</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>61</v>
@@ -1204,10 +1204,10 @@
         <v>1.0</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>58</v>
@@ -1216,7 +1216,7 @@
         <v>59</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>61</v>
@@ -1227,10 +1227,10 @@
         <v>1.0</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>58</v>
@@ -1239,7 +1239,7 @@
         <v>59</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>61</v>
@@ -1250,10 +1250,10 @@
         <v>1.0</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>58</v>
@@ -1262,7 +1262,7 @@
         <v>59</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>61</v>
@@ -1273,10 +1273,10 @@
         <v>2.0</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>58</v>
@@ -1285,7 +1285,7 @@
         <v>59</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>61</v>
@@ -1296,20 +1296,20 @@
         <v>1.0</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
@@ -1317,20 +1317,20 @@
         <v>1.0</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
@@ -1338,20 +1338,20 @@
         <v>1.0</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
@@ -1359,22 +1359,22 @@
         <v>1.0</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
@@ -1382,20 +1382,20 @@
         <v>1.0</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
@@ -1403,20 +1403,20 @@
         <v>1.0</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="32" ht="12.75" customHeight="1"/>

</xml_diff>